<commit_message>
Added "Name" column to results masterfile
</commit_message>
<xml_diff>
--- a/data/Designs/Archive/RBSrandomPWM + bandit.xlsx
+++ b/data/Designs/Archive/RBSrandomPWM + bandit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOL428\OneDrive - CSIRO\Collaborations\[SOLARIS]\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOL428\Documents\GitHub\SynbioML\data\Designs\Archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{0BB47869-CAC5-450A-A897-3D9E48780543}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{C5CC1818-B7C4-452F-ABEE-4FED2A6844ED}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C1EF9E-7F38-4D9B-A396-B99DAAFD7F30}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4032" yWindow="2508" windowWidth="23040" windowHeight="12156" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequences" sheetId="1" r:id="rId1"/>
@@ -938,8 +938,8 @@
   </sheetPr>
   <dimension ref="A1:L91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>